<commit_message>
BR : Added feature to add multiple interest
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="347">
   <si>
     <t>AASC Limited ( HLB Vietnam )&amp;</t>
   </si>
@@ -1044,6 +1044,9 @@
   </si>
   <si>
     <t>helloworld@gmail.com</t>
+  </si>
+  <si>
+    <t>Tax,Advisory</t>
   </si>
   <si>
     <t>polar</t>
@@ -1103,7 +1106,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -1111,7 +1114,13 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1424,7 +1433,7 @@
   <cols>
     <col min="1" max="1" style="2" width="19.14785714285714" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="2" width="19.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="32.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="32.71928571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="2" width="47.43357142857143" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="2" width="9.719285714285713" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="2" width="33.57642857142857" customWidth="1" bestFit="1"/>
@@ -1437,7 +1446,7 @@
       <c r="B1" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>336</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1457,7 +1466,7 @@
       <c r="B2" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>342</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1467,18 +1476,18 @@
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>4</v>
+        <v>343</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="C3" s="3" t="s">
         <v>345</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>346</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>

</xml_diff>